<commit_message>
Use Drogon for cpp
</commit_message>
<xml_diff>
--- a/illustration.xlsx
+++ b/illustration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\maxreq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884E81E3-2498-40E0-BC2D-129A3B5791AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B216DA32-03E9-4292-BA0C-F18C81D5AB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>node.js</t>
-  </si>
-  <si>
-    <t>.NET Core</t>
   </si>
   <si>
     <t>Rust</t>
@@ -57,6 +54,12 @@
   </si>
   <si>
     <t>Java</t>
+  </si>
+  <si>
+    <t>C#</t>
+  </si>
+  <si>
+    <t>C++</t>
   </si>
 </sst>
 </file>
@@ -257,9 +260,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$7</c:f>
+              <c:f>Feuil1!$A$2:$A$8</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>PHP</c:v>
                 </c:pt>
@@ -273,9 +276,12 @@
                   <c:v>Java</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>.NET Core</c:v>
+                  <c:v>C++</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>C#</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Rust</c:v>
                 </c:pt>
               </c:strCache>
@@ -283,10 +289,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$B$7</c:f>
+              <c:f>Feuil1!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1227</c:v>
                 </c:pt>
@@ -300,9 +306,12 @@
                   <c:v>4526</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>5652</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>7417</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>17887</c:v>
                 </c:pt>
               </c:numCache>
@@ -1062,7 +1071,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1408,9 +1417,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96EDF2E-1656-4DA5-843F-3F6E7E24D056}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -1418,12 +1427,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>1227</v>
@@ -1431,7 +1440,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1935</v>
@@ -1447,7 +1456,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>4526</v>
@@ -1455,17 +1464,25 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>7417</v>
+        <v>5652</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B7">
+        <v>7417</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>17887</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change test environment for PHP and node.js
</commit_message>
<xml_diff>
--- a/illustration.xlsx
+++ b/illustration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\maxreq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0511EDCB-0CA3-439B-9055-77C84F17DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A92AB3-7B15-4351-B509-DC8C8C5ACB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="17280" windowHeight="11858" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
+    <workbookView xWindow="6240" yWindow="1845" windowWidth="21600" windowHeight="12360" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -270,10 +270,10 @@
                   <c:v>PHP</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>node.js</c:v>
+                  <c:v>Python</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Python</c:v>
+                  <c:v>node.js</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>Java</c:v>
@@ -300,13 +300,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1227</c:v>
+                  <c:v>2065</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2076</c:v>
+                  <c:v>2112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2112</c:v>
+                  <c:v>2267</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>4526</c:v>
@@ -1429,41 +1429,41 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1227</v>
+        <v>2065</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>2076</v>
+      <c r="B4">
+        <v>2267</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>2112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>4526</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>5652</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>7417</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>12049</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Add java minimal API
</commit_message>
<xml_diff>
--- a/illustration.xlsx
+++ b/illustration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\maxreq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40ECAD96-48D5-446F-9626-63FB50E903F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FD07A36-C447-4DE5-9FE1-EC08A3EBFCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>node.js</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Java</t>
   </si>
   <si>
-    <t>C++</t>
-  </si>
-  <si>
     <t>Go</t>
   </si>
   <si>
@@ -66,6 +63,12 @@
   </si>
   <si>
     <t>PHP (CGI)</t>
+  </si>
+  <si>
+    <t>Java Minial API</t>
+  </si>
+  <si>
+    <t>C++ (*)</t>
   </si>
 </sst>
 </file>
@@ -266,9 +269,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$2:$A$10</c:f>
+              <c:f>Feuil1!$A$2:$A$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>PHP (CGI)</c:v>
                 </c:pt>
@@ -279,21 +282,24 @@
                   <c:v>Java</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Java Minial API</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>Python</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>C++</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>C++ (*)</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>C# - Controller</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>C# - Minimal API</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>Go</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Rust</c:v>
                 </c:pt>
               </c:strCache>
@@ -301,10 +307,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$2:$B$10</c:f>
+              <c:f>Feuil1!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2072</c:v>
                 </c:pt>
@@ -315,21 +321,24 @@
                   <c:v>3235</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>3805</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4564</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>5920</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>6508</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>7401</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>12694</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>18563</c:v>
                 </c:pt>
               </c:numCache>
@@ -1089,7 +1098,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>723900</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1435,10 +1444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96EDF2E-1656-4DA5-843F-3F6E7E24D056}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1450,7 +1459,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>2072</v>
@@ -1474,55 +1483,63 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>4564</v>
+        <v>3805</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>5920</v>
+        <v>4564</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>6508</v>
+        <v>5920</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>7401</v>
+        <v>6508</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>12694</v>
+        <v>7401</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>12694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>18563</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B10">
-    <sortCondition ref="B10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B11">
+    <sortCondition ref="B11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
several improvements and unification
</commit_message>
<xml_diff>
--- a/illustration.xlsx
+++ b/illustration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\dev2\AI\maxreq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA05915-1396-4479-B121-E08F9B91F9B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBBBF8F-19EF-4B57-A2C2-8A64DEAA0B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
+    <workbookView xWindow="1230" yWindow="1230" windowWidth="21600" windowHeight="12915" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>node.js</t>
   </si>
@@ -56,9 +56,6 @@
     <t>PHP (CGI)</t>
   </si>
   <si>
-    <t>Java Minial API</t>
-  </si>
-  <si>
     <t>C++ (*)</t>
   </si>
   <si>
@@ -75,6 +72,18 @@
   </si>
   <si>
     <t>Test date</t>
+  </si>
+  <si>
+    <t>Bun (Typescript)</t>
+  </si>
+  <si>
+    <t>no_db</t>
+  </si>
+  <si>
+    <t>Run each 5 time and keep the best one</t>
+  </si>
+  <si>
+    <t>Java Minimal API</t>
   </si>
 </sst>
 </file>
@@ -268,9 +277,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Feuil1!$A$1:$A$12</c:f>
+              <c:f>Feuil1!$A$1:$A$13</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>Request/second</c:v>
                 </c:pt>
@@ -281,41 +290,44 @@
                   <c:v>node.js</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>Python</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>C# - Controller .NET 9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>C# - Minimal API .NET 9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>C++ (*)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Rust Axum</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Rust Actix</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>Java</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>Java Minial API</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>C# - Controller .NET 9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Python</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>C# - Minimal API .NET 9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>C++ (*)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Rust Axum</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>Rust Actix</c:v>
+                  <c:v>Bun (Typescript)</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Java Minimal API</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Feuil1!$B$1:$B$12</c:f>
+              <c:f>Feuil1!$B$1:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="1">
                   <c:v>2072</c:v>
                 </c:pt>
@@ -323,31 +335,34 @@
                   <c:v>2382</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3235</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3805</c:v>
+                  <c:v>4500</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4500</c:v>
+                  <c:v>5371</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4564</c:v>
+                  <c:v>5920</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5371</c:v>
+                  <c:v>7939</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5920</c:v>
+                  <c:v>8233</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6028</c:v>
+                  <c:v>9954</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6335</c:v>
+                  <c:v>10111</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>16596</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32600</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1098,15 +1113,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1452,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96EDF2E-1656-4DA5-843F-3F6E7E24D056}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,15 +1478,18 @@
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1479,7 +1497,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1487,96 +1505,142 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>3235</v>
+        <v>3600</v>
+      </c>
+      <c r="C4">
+        <v>4287</v>
+      </c>
+      <c r="D4" s="1">
+        <v>45922</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>4500</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>5371</v>
+      </c>
+      <c r="D6" s="1">
+        <v>45920</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>3805</v>
+      <c r="B7">
+        <v>5920</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>4500</v>
-      </c>
-      <c r="C6" s="1">
-        <v>45920</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>7939</v>
+      </c>
+      <c r="C8">
+        <v>8904</v>
+      </c>
+      <c r="D8" s="1">
+        <v>45921</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>4564</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>5371</v>
-      </c>
-      <c r="C8" s="1">
-        <v>45920</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>5920</v>
+        <v>8233</v>
+      </c>
+      <c r="C9">
+        <v>9277</v>
+      </c>
+      <c r="D9" s="1">
+        <v>45921</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>6028</v>
-      </c>
-      <c r="C10" s="1">
-        <v>45920</v>
+        <v>9954</v>
+      </c>
+      <c r="C10">
+        <v>32531</v>
+      </c>
+      <c r="D10" s="1">
+        <v>45921</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>6335</v>
-      </c>
-      <c r="C11" s="1">
-        <v>45920</v>
+        <v>10111</v>
+      </c>
+      <c r="C11">
+        <v>20252</v>
+      </c>
+      <c r="D11" s="1">
+        <v>45921</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
       <c r="B12">
         <v>16596</v>
       </c>
-      <c r="C12" s="1">
-        <v>45920</v>
+      <c r="C12">
+        <v>48785</v>
+      </c>
+      <c r="D12" s="1">
+        <v>45921</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>32600</v>
+      </c>
+      <c r="C13">
+        <v>39167</v>
+      </c>
+      <c r="D13" s="1">
+        <v>45921</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B12">
-    <sortCondition ref="B3:B12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
+    <sortCondition ref="B2:B13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Working on CppServer compilation
</commit_message>
<xml_diff>
--- a/illustration.xlsx
+++ b/illustration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\dev2\AI\maxreq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88322B61-B5EC-4AC3-A3D3-07175D2F9B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF825CB9-3D43-4609-91B2-7BF9FC28C8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" activeTab="1" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ryzen 7" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -219,7 +219,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -587,7 +587,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -657,7 +657,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2674,16 +2674,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96EDF2E-1656-4DA5-843F-3F6E7E24D056}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>2072</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>45920</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>45920</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>5920</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>45921</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>45921</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>45921</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>45921</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -2824,7 +2824,7 @@
         <v>45921</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>45921</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2857,16 +2857,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D309CC-6B37-4C27-9D09-BA240EF5EF8A}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2931,7 +2931,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -2995,7 +2995,7 @@
       </c>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -3009,28 +3009,28 @@
         <v>45922</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
C++ version with ASIO CppServer. We can certainly improve a bit.
</commit_message>
<xml_diff>
--- a/illustration.xlsx
+++ b/illustration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\dev2\AI\maxreq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF825CB9-3D43-4609-91B2-7BF9FC28C8AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9BA3F3-EDD9-4524-A656-84B7E0971DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="13545" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
   </bookViews>
   <sheets>
     <sheet name="Ryzen 7" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>node.js</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t>Jave Manimal API oracle 17</t>
+  </si>
+  <si>
+    <t>C++ dragon</t>
+  </si>
+  <si>
+    <t>C++ asio CppServer</t>
   </si>
 </sst>
 </file>
@@ -297,9 +303,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Ryzen 7'!$A$1:$A$13</c:f>
+              <c:f>'Ryzen 7'!$A$1:$A$14</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>Request/second</c:v>
                 </c:pt>
@@ -319,24 +325,27 @@
                   <c:v>C# - Minimal API .NET 9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>C++ (*)</c:v>
+                  <c:v>C++ dragon</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>C++ asio CppServer</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>Rust Axum</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>Rust Actix</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>Java</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>Bun (Typescript)</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>Go</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>Java Minimal API</c:v>
                 </c:pt>
               </c:strCache>
@@ -344,10 +353,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ryzen 7'!$B$1:$B$13</c:f>
+              <c:f>'Ryzen 7'!$B$1:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="1">
                   <c:v>2072</c:v>
                 </c:pt>
@@ -367,21 +376,24 @@
                   <c:v>5920</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>7084</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>7939</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>8233</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>9954</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>10111</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>16596</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>32600</c:v>
                 </c:pt>
               </c:numCache>
@@ -2283,7 +2295,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2672,10 +2684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D96EDF2E-1656-4DA5-843F-3F6E7E24D056}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2748,7 +2760,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>5920</v>
@@ -2756,27 +2768,27 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B8">
-        <v>7939</v>
+        <v>7084</v>
       </c>
       <c r="C8">
-        <v>8904</v>
+        <v>10479</v>
       </c>
       <c r="D8" s="1">
-        <v>45921</v>
+        <v>45933</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>8233</v>
+        <v>7939</v>
       </c>
       <c r="C9">
-        <v>9277</v>
+        <v>8904</v>
       </c>
       <c r="D9" s="1">
         <v>45921</v>
@@ -2784,13 +2796,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>9954</v>
+        <v>8233</v>
       </c>
       <c r="C10">
-        <v>32531</v>
+        <v>9277</v>
       </c>
       <c r="D10" s="1">
         <v>45921</v>
@@ -2798,13 +2810,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>10111</v>
+        <v>9954</v>
       </c>
       <c r="C11">
-        <v>20252</v>
+        <v>32531</v>
       </c>
       <c r="D11" s="1">
         <v>45921</v>
@@ -2812,13 +2824,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>16596</v>
+        <v>10111</v>
       </c>
       <c r="C12">
-        <v>48785</v>
+        <v>20252</v>
       </c>
       <c r="D12" s="1">
         <v>45921</v>
@@ -2826,26 +2838,40 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B13">
-        <v>32600</v>
+        <v>16596</v>
       </c>
       <c r="C13">
-        <v>39167</v>
+        <v>48785</v>
       </c>
       <c r="D13" s="1">
         <v>45921</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>32600</v>
+      </c>
+      <c r="C14">
+        <v>39167</v>
+      </c>
+      <c r="D14" s="1">
+        <v>45921</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
-    <sortCondition ref="B2:B13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D14">
+    <sortCondition ref="B2:B14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update performance comparison details in README and LinkedIn post; add Debian illustration
</commit_message>
<xml_diff>
--- a/illustration.xlsx
+++ b/illustration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\dev2\AI\maxreq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35095295-687E-4AE3-8717-77F0F2A86AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A738F7-05B0-4C6B-89C8-C315D9828224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13996" activeTab="2" xr2:uid="{118BFD8F-90CA-4E6C-93EF-A5ACB82B758A}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="OVH" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">OVH!$A$3:$D$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">OVH!$A$3:$D$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>node.js</t>
   </si>
@@ -171,13 +171,33 @@
   <si>
     <t>Python (ASGI Uvicorn)</t>
   </si>
+  <si>
+    <t>NodeJS (pm2 + nginx)</t>
+  </si>
+  <si>
+    <t>Fastest/line</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -193,7 +213,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -201,13 +221,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1438,11 +1475,11 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>OVH!$B$4:$B$20</c:f>
+              <c:f>OVH!$B$5:$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>Javamini Azul native (1)</c:v>
+                  <c:v>NodeJS (pm2 + nginx)</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Python (ASGI Uvicorn)</c:v>
@@ -1497,67 +1534,215 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>OVH!$D$4:$D$20</c:f>
+              <c:f>OVH!$C$5:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>268</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3159</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4892</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5558</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5702</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6131</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>6442</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7229</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>7798</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10496</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10967</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13093</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13620</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15669</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16203</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>18095</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>19303</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-F956-4908-B573-FAC9977D3D45}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:alpha val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>OVH!$B$5:$B$21</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>NodeJS (pm2 + nginx)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Python (ASGI Uvicorn)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Java Temurin Docker</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Java Graal Docker</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Java Azul Docker</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Java Graal native</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>PHP (Nginx + PHP-FPM)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Java Azul native</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Java Temurin native</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Bun (Javascript)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Go</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Javamini Temurin native</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>C# - Controller .NET 9</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Javamini Graal native</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>C# - Minimal API .NET 9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Rust</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Rust Actix</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>OVH!$D$5:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1238</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3159</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4892</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5558</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5702</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6131</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7229</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7798</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10496</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10967</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13093</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13620</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15669</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16203</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18095</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19303</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3874-4318-8145-57879945029C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1716,21 +1901,34 @@
     <a:gradFill flip="none" rotWithShape="1">
       <a:gsLst>
         <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:shade val="30000"/>
+            <a:satMod val="115000"/>
+          </a:schemeClr>
         </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
+        <a:gs pos="50000">
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:shade val="67500"/>
+            <a:satMod val="115000"/>
+          </a:schemeClr>
         </a:gs>
         <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:shade val="100000"/>
+            <a:satMod val="115000"/>
           </a:schemeClr>
         </a:gs>
       </a:gsLst>
       <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        <a:fillToRect l="100000" b="100000"/>
       </a:path>
-      <a:tileRect/>
+      <a:tileRect t="-100000" r="-100000"/>
     </a:gradFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -3557,7 +3755,7 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>566737</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>51874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4291,10 +4489,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C568D5-A42A-4923-9916-9948BE1E3A2A}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4330,16 +4528,30 @@
       <c r="D3" t="s">
         <v>28</v>
       </c>
+      <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>45961</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D4">
         <v>268</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E20" si="0">$D$21/D4</f>
+        <v>72.026119402985074</v>
+      </c>
+      <c r="F4" t="str">
+        <f>_xlfn.CONCAT(D4," (x",ROUND(E4,2),")")</f>
+        <v>268 (x72,03)</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -4347,21 +4559,37 @@
         <v>45961</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5">
-        <v>3159</v>
+        <v>1238</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>15.592084006462036</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F21" si="1">_xlfn.CONCAT(D5," (x",ROUND(E5,2),")")</f>
+        <v>1238 (x15,59)</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
-        <v>45959</v>
+        <v>45961</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="D6">
-        <v>4892</v>
+        <v>3159</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>6.1104779993668883</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>3159 (x6,11)</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -4369,10 +4597,18 @@
         <v>45959</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D7">
-        <v>5558</v>
+        <v>4892</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>3.9458299264104659</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>4892 (x3,95)</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -4380,21 +4616,37 @@
         <v>45959</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8">
-        <v>5702</v>
+        <v>5558</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4730118747750991</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>5558 (x3,47)</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
-        <v>45961</v>
+        <v>45959</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9">
-        <v>6131</v>
+        <v>5702</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>3.3853034023149773</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>5702 (x3,39)</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -4402,10 +4654,18 @@
         <v>45961</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D10">
-        <v>6442</v>
+        <v>6131</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>3.1484260316424728</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>6131 (x3,15)</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
@@ -4413,10 +4673,18 @@
         <v>45961</v>
       </c>
       <c r="B11" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D11">
-        <v>7229</v>
+        <v>6442</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>2.9964296802235331</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="1"/>
+        <v>6442 (x3)</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -4424,10 +4692,18 @@
         <v>45961</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D12">
-        <v>7798</v>
+        <v>7229</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>2.6702171807995572</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="1"/>
+        <v>7229 (x2,67)</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -4435,10 +4711,18 @@
         <v>45961</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D13">
-        <v>10496</v>
+        <v>7798</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>2.475378302128751</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="1"/>
+        <v>7798 (x2,48)</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
@@ -4446,10 +4730,18 @@
         <v>45961</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D14">
-        <v>10967</v>
+        <v>10496</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>1.8390815548780488</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="1"/>
+        <v>10496 (x1,84)</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
@@ -4457,10 +4749,18 @@
         <v>45961</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>13093</v>
+        <v>10967</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>1.7600984772499315</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="1"/>
+        <v>10967 (x1,76)</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
@@ -4468,66 +4768,126 @@
         <v>45961</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D16">
-        <v>13620</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+        <v>13093</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4742992438707707</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="1"/>
+        <v>13093 (x1,47)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>45961</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="D17">
-        <v>15669</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+        <v>13620</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>1.4172540381791483</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="1"/>
+        <v>13620 (x1,42)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>45961</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="D18">
-        <v>16203</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+        <v>15669</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2319229050992406</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="1"/>
+        <v>15669 (x1,23)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>45961</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D19">
-        <v>18095</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>16203</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1913225945812504</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="1"/>
+        <v>16203 (x1,19)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>45961</v>
       </c>
       <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20">
+        <v>18095</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0667587731417518</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="1"/>
+        <v>18095 (x1,07)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="D20">
+      <c r="D21">
         <v>19303</v>
       </c>
+      <c r="E21" s="3">
+        <f>$D$21/D21</f>
+        <v>1</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="1"/>
+        <v>19303 (x1)</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:D20" xr:uid="{09C568D5-A42A-4923-9916-9948BE1E3A2A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D20">
-      <sortCondition ref="D3:D20"/>
+  <autoFilter ref="A3:D21" xr:uid="{09C568D5-A42A-4923-9916-9948BE1E3A2A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D21">
+      <sortCondition ref="D3:D21"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H20">
-    <sortCondition descending="1" ref="D4:D20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H21">
+    <sortCondition descending="1" ref="D4:D21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>